<commit_message>
Microplan Generated - Function Works Fine
</commit_message>
<xml_diff>
--- a/__test__/ProcessFiles/303 MDA Mircorplan.xlsx
+++ b/__test__/ProcessFiles/303 MDA Mircorplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\MDA Modified\MDA 2025 HOUSE TO HOUSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\appDev\plansheetExcel_Working Files\plansheetExcel\__test__\ProcessFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -487,38 +487,8 @@
   </cellStyleXfs>
   <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -533,79 +503,109 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,543 +890,609 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="3"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="32"/>
     </row>
     <row r="2" spans="1:15" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="6"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="35"/>
     </row>
     <row r="3" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="12" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14" t="s">
+      <c r="L3" s="3"/>
+      <c r="M3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="16"/>
+      <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="17" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="19"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="42"/>
     </row>
     <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="17" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="19"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="42"/>
     </row>
     <row r="6" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="21" t="s">
+      <c r="C6" s="29"/>
+      <c r="D6" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="23" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="21" t="s">
+      <c r="G6" s="27"/>
+      <c r="H6" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="21" t="s">
+      <c r="I6" s="29"/>
+      <c r="J6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="21" t="s">
+      <c r="K6" s="29"/>
+      <c r="L6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="21" t="s">
+      <c r="M6" s="29"/>
+      <c r="N6" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="22"/>
+      <c r="O6" s="29"/>
     </row>
     <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="26"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="19"/>
     </row>
     <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27" t="s">
+      <c r="E8" s="19"/>
+      <c r="F8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27" t="s">
+      <c r="G8" s="19"/>
+      <c r="H8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27" t="s">
+      <c r="I8" s="19"/>
+      <c r="J8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="26"/>
-      <c r="L8" s="27" t="s">
+      <c r="K8" s="19"/>
+      <c r="L8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="26"/>
-      <c r="N8" s="27" t="s">
+      <c r="M8" s="19"/>
+      <c r="N8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="26"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27" t="s">
+      <c r="C9" s="19"/>
+      <c r="D9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="27" t="s">
+      <c r="G9" s="19"/>
+      <c r="H9" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27" t="s">
+      <c r="I9" s="19"/>
+      <c r="J9" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27" t="s">
+      <c r="K9" s="19"/>
+      <c r="L9" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="M9" s="26"/>
-      <c r="N9" s="25" t="s">
+      <c r="M9" s="19"/>
+      <c r="N9" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="O9" s="26"/>
+      <c r="O9" s="19"/>
     </row>
     <row r="10" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="20">
         <v>21</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="D10" s="25">
+      <c r="C10" s="19"/>
+      <c r="D10" s="20">
         <v>21</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="25">
+      <c r="E10" s="19"/>
+      <c r="F10" s="20">
         <v>21</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="25">
+      <c r="G10" s="19"/>
+      <c r="H10" s="20">
         <v>21</v>
       </c>
-      <c r="I10" s="26"/>
-      <c r="J10" s="25">
+      <c r="I10" s="19"/>
+      <c r="J10" s="20">
         <v>21</v>
       </c>
-      <c r="K10" s="26"/>
-      <c r="L10" s="25">
+      <c r="K10" s="19"/>
+      <c r="L10" s="20">
         <v>21</v>
       </c>
-      <c r="M10" s="26"/>
-      <c r="N10" s="25">
+      <c r="M10" s="19"/>
+      <c r="N10" s="20">
         <v>21</v>
       </c>
-      <c r="O10" s="26"/>
+      <c r="O10" s="19"/>
     </row>
     <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="26"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="19"/>
     </row>
     <row r="12" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="31"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="23"/>
     </row>
     <row r="13" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="32" t="s">
+      <c r="C13" s="25"/>
+      <c r="D13" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="23" t="s">
+      <c r="E13" s="25"/>
+      <c r="F13" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="32" t="s">
+      <c r="G13" s="27"/>
+      <c r="H13" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="33"/>
-      <c r="J13" s="32" t="s">
+      <c r="I13" s="25"/>
+      <c r="J13" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="K13" s="33"/>
-      <c r="L13" s="32" t="s">
+      <c r="K13" s="25"/>
+      <c r="L13" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="M13" s="33"/>
-      <c r="N13" s="32" t="s">
+      <c r="M13" s="25"/>
+      <c r="N13" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="O13" s="33"/>
+      <c r="O13" s="25"/>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="26"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="19"/>
     </row>
     <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27" t="s">
+      <c r="C15" s="19"/>
+      <c r="D15" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="25" t="s">
+      <c r="E15" s="19"/>
+      <c r="F15" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27" t="s">
+      <c r="G15" s="19"/>
+      <c r="H15" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27" t="s">
+      <c r="I15" s="19"/>
+      <c r="J15" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="K15" s="26"/>
-      <c r="L15" s="27" t="s">
+      <c r="K15" s="19"/>
+      <c r="L15" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M15" s="26"/>
-      <c r="N15" s="27" t="s">
+      <c r="M15" s="19"/>
+      <c r="N15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="O15" s="26"/>
+      <c r="O15" s="19"/>
     </row>
     <row r="16" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="34" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="34" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36" t="s">
+      <c r="G16" s="15"/>
+      <c r="H16" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="34" t="s">
+      <c r="I16" s="15"/>
+      <c r="J16" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="K16" s="35"/>
-      <c r="L16" s="37" t="s">
+      <c r="K16" s="15"/>
+      <c r="L16" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="M16" s="35"/>
-      <c r="N16" s="34" t="s">
+      <c r="M16" s="15"/>
+      <c r="N16" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="O16" s="35"/>
+      <c r="O16" s="15"/>
     </row>
     <row r="17" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="10">
         <v>21</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="28">
+      <c r="C17" s="11"/>
+      <c r="D17" s="10">
         <v>22</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="28">
+      <c r="E17" s="11"/>
+      <c r="F17" s="10">
         <v>22</v>
       </c>
-      <c r="G17" s="38"/>
-      <c r="H17" s="28">
+      <c r="G17" s="11"/>
+      <c r="H17" s="10">
         <v>22</v>
       </c>
-      <c r="I17" s="38"/>
-      <c r="J17" s="28">
+      <c r="I17" s="11"/>
+      <c r="J17" s="10">
         <v>22</v>
       </c>
-      <c r="K17" s="38"/>
-      <c r="L17" s="28">
+      <c r="K17" s="11"/>
+      <c r="L17" s="10">
         <v>22</v>
       </c>
-      <c r="M17" s="38"/>
-      <c r="N17" s="28">
+      <c r="M17" s="11"/>
+      <c r="N17" s="10">
         <v>22</v>
       </c>
-      <c r="O17" s="38"/>
+      <c r="O17" s="11"/>
     </row>
     <row r="18" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="38"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="11"/>
     </row>
     <row r="19" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
     </row>
     <row r="23" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="A20:O20"/>
-    <mergeCell ref="A23:O23"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:O4"/>
+    <mergeCell ref="D5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="A12:O12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
@@ -1441,78 +1507,15 @@
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="A12:O12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:O4"/>
-    <mergeCell ref="D5:O5"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="A20:O20"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="L18:M18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>